<commit_message>
Normalizacion de RegistroAutomotorDB | DER FINAL
</commit_message>
<xml_diff>
--- a/Unidad_3_Diseno_DBs/10_Normalizamos_RegistroAutomotorDB/Normalizamos RegistroAutomotorDB.xlsx
+++ b/Unidad_3_Diseno_DBs/10_Normalizamos_RegistroAutomotorDB/Normalizamos RegistroAutomotorDB.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\MaxiPrograma-Database\Unidad_3_Diseno_DBs\10_Normalizamos_RegistroAutomotorDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A331589-0D90-47A9-A389-BD17D0138E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3890D04E-7B8C-40AC-9394-4C4F28DBECC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F11CE39-A58D-4EFD-B45E-905AD35642EF}"/>
+    <workbookView xWindow="20820" yWindow="3180" windowWidth="15810" windowHeight="11385" activeTab="1" xr2:uid="{9F11CE39-A58D-4EFD-B45E-905AD35642EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vehiculos" sheetId="1" r:id="rId1"/>
+    <sheet name="Mantenimiento" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="81">
   <si>
     <t>Ford</t>
   </si>
@@ -172,6 +174,114 @@
   </si>
   <si>
     <t>QQQ111</t>
+  </si>
+  <si>
+    <t>Seguimos</t>
+  </si>
+  <si>
+    <t>IdTipoVehiculo</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Taller</t>
+  </si>
+  <si>
+    <t>TipoMantenimiento</t>
+  </si>
+  <si>
+    <t>Insumos</t>
+  </si>
+  <si>
+    <t>Mecanico</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>IdVehiculos</t>
+  </si>
+  <si>
+    <t>Beto's Cars</t>
+  </si>
+  <si>
+    <t>Pepe Motors</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Cambio de amortiguadores</t>
+  </si>
+  <si>
+    <t>Aceite, filtro nafta, filtro habitaculo, filtro motor</t>
+  </si>
+  <si>
+    <t>Amortiguadores marca JJ, vielas, rulemanes</t>
+  </si>
+  <si>
+    <t>Beto Jr</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>Avenida 123</t>
+  </si>
+  <si>
+    <t>Calle Plana 333</t>
+  </si>
+  <si>
+    <t>Talleres</t>
+  </si>
+  <si>
+    <t>IdMecanico</t>
+  </si>
+  <si>
+    <t>Mecanicos</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Marcas</t>
+  </si>
+  <si>
+    <t>TipoMantenimientos</t>
+  </si>
+  <si>
+    <t>IdInsumo</t>
+  </si>
+  <si>
+    <t>Aceite</t>
+  </si>
+  <si>
+    <t>Filtro Nafta</t>
+  </si>
+  <si>
+    <t>Filtro Habitaculo</t>
+  </si>
+  <si>
+    <t>Filtro Motor</t>
+  </si>
+  <si>
+    <t>Amortiguadores JJ</t>
+  </si>
+  <si>
+    <t>Viela</t>
+  </si>
+  <si>
+    <t>Rulemanes</t>
+  </si>
+  <si>
+    <t>2FN</t>
+  </si>
+  <si>
+    <t>IdMantenimiento</t>
+  </si>
+  <si>
+    <t>Insumos.Matenimiento | Tabla intermedia</t>
   </si>
 </sst>
 </file>
@@ -211,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,8 +358,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -538,11 +660,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,6 +775,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,6 +852,55 @@
         <a:xfrm>
           <a:off x="228600" y="438150"/>
           <a:ext cx="1486107" cy="2629267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>588819</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>56025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5CBFFC0-E80D-46D3-B60D-E17ADD552104}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="0"/>
+          <a:ext cx="3636818" cy="5390025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1002,15 +1209,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A485C05-513C-4172-995B-AE7C87C0D4F2}">
-  <dimension ref="C2:N37"/>
+  <dimension ref="C2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1155,529 +1363,683 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E9" s="4"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="18" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="20"/>
+      <c r="M11" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="22"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="4"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="20"/>
+      <c r="M12" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="D13" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="26">
+        <v>1</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>1</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="26">
+        <v>1</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="26">
+        <v>1</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="26">
+        <v>1</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D18" s="24">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="24">
+        <v>2</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="24">
+        <v>2</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="24">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="24">
+        <v>2</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="26">
+        <v>3</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="26">
+        <v>3</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="26">
+        <v>3</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="26">
+        <v>3</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" s="26">
+        <v>3</v>
+      </c>
+      <c r="M19" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="24">
+        <v>4</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="24">
+        <v>4</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="24">
+        <v>4</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="24">
+        <v>4</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="26">
+        <v>5</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="26">
+        <v>5</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D24" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="1" t="s">
+      <c r="G24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="1" t="s">
+      <c r="H24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2014</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1</v>
+      </c>
+      <c r="J25" s="4">
+        <v>150000</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="4">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2018</v>
+      </c>
+      <c r="I26" s="4">
+        <v>2</v>
+      </c>
+      <c r="J26" s="4">
+        <v>25000</v>
+      </c>
+      <c r="K26" s="4">
+        <v>2</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="30">
+        <v>3</v>
+      </c>
+      <c r="F27" s="31">
+        <v>1</v>
+      </c>
+      <c r="G27" s="32">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E30" s="35"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D31" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="36"/>
+      <c r="F31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4">
+        <v>2014</v>
+      </c>
+      <c r="I32" s="4">
+        <v>1</v>
+      </c>
+      <c r="J32" s="4">
+        <v>150000</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4">
+        <v>2</v>
+      </c>
+      <c r="H33" s="4">
+        <v>2018</v>
+      </c>
+      <c r="I33" s="4">
+        <v>2</v>
+      </c>
+      <c r="J33" s="4">
+        <v>25000</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F34" s="37">
+        <v>3</v>
+      </c>
+      <c r="G34" s="37">
+        <v>1</v>
+      </c>
+      <c r="H34" s="37">
+        <v>2016</v>
+      </c>
+      <c r="I34" s="37">
+        <v>3</v>
+      </c>
+      <c r="J34" s="37">
+        <v>30000</v>
+      </c>
+      <c r="K34" s="37">
+        <v>2</v>
+      </c>
+      <c r="L34" s="37">
+        <v>1</v>
+      </c>
+      <c r="M34" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="N34" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="18" t="s">
+      <c r="J38" s="16"/>
+      <c r="K38" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="19"/>
-      <c r="M13" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="7"/>
-      <c r="E14" s="6" t="s">
+      <c r="L38" s="19"/>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E39" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="6" t="s">
+      <c r="F39" s="11"/>
+      <c r="G39" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="15" t="s">
+      <c r="H39" s="5"/>
+      <c r="I39" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="8" t="s">
+      <c r="J39" s="17"/>
+      <c r="K39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="20"/>
-      <c r="M14" s="8" t="s">
+      <c r="L39" s="20"/>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="17"/>
+      <c r="K40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="20"/>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G42" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D45" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="36"/>
+      <c r="F45" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="7"/>
-      <c r="E15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="14" t="s">
+      <c r="G45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="20"/>
-      <c r="M15" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="26">
-        <v>1</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="26">
-        <v>1</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="26">
-        <v>1</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="26">
-        <v>1</v>
-      </c>
-      <c r="K18" s="27" t="s">
+      <c r="J45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4">
+        <v>2014</v>
+      </c>
+      <c r="I46" s="4">
+        <v>1</v>
+      </c>
+      <c r="J46" s="4">
+        <v>150000</v>
+      </c>
+      <c r="K46" s="4">
+        <v>1</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4">
+        <v>2</v>
+      </c>
+      <c r="G47" s="4">
+        <v>2</v>
+      </c>
+      <c r="H47" s="4">
+        <v>2018</v>
+      </c>
+      <c r="I47" s="4">
+        <v>2</v>
+      </c>
+      <c r="J47" s="4">
+        <v>25000</v>
+      </c>
+      <c r="K47" s="4">
+        <v>2</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M47" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F48" s="37">
         <v>3</v>
       </c>
-      <c r="L18" s="26">
-        <v>1</v>
-      </c>
-      <c r="M18" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="24">
-        <v>2</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="24">
-        <v>2</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="24">
-        <v>2</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="24">
-        <v>2</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="24">
-        <v>2</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="26">
+      <c r="G48" s="37">
+        <v>1</v>
+      </c>
+      <c r="H48" s="37">
+        <v>2016</v>
+      </c>
+      <c r="I48" s="37">
         <v>3</v>
       </c>
-      <c r="E20" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="26">
-        <v>3</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="26">
-        <v>3</v>
-      </c>
-      <c r="I20" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="26">
-        <v>3</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" s="26">
-        <v>3</v>
-      </c>
-      <c r="M20" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D21" s="24">
-        <v>4</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="24">
-        <v>4</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="24">
-        <v>4</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="24">
-        <v>4</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D22" s="26">
-        <v>5</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="26">
-        <v>5</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D27" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E28" s="4">
-        <v>1</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4">
-        <v>2014</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4">
-        <v>150000</v>
-      </c>
-      <c r="K28" s="4">
-        <v>1</v>
-      </c>
-      <c r="L28" s="4">
-        <v>1</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E29" s="4">
-        <v>2</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1</v>
-      </c>
-      <c r="G29" s="4">
-        <v>2</v>
-      </c>
-      <c r="H29" s="4">
-        <v>2018</v>
-      </c>
-      <c r="I29" s="4">
-        <v>2</v>
-      </c>
-      <c r="J29" s="4">
-        <v>25000</v>
-      </c>
-      <c r="K29" s="4">
-        <v>2</v>
-      </c>
-      <c r="L29" s="4">
-        <v>1</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N29" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="30">
-        <v>3</v>
-      </c>
-      <c r="F30" s="31">
-        <v>1</v>
-      </c>
-      <c r="G30" s="32">
-        <v>5</v>
-      </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E33" s="35"/>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D34" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E35" s="4"/>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="4">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4">
-        <v>2014</v>
-      </c>
-      <c r="I35" s="4">
-        <v>1</v>
-      </c>
-      <c r="J35" s="4">
-        <v>150000</v>
-      </c>
-      <c r="K35" s="4">
-        <v>1</v>
-      </c>
-      <c r="L35" s="4">
-        <v>1</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N35" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E36" s="4"/>
-      <c r="F36" s="4">
-        <v>2</v>
-      </c>
-      <c r="G36" s="4">
-        <v>2</v>
-      </c>
-      <c r="H36" s="4">
-        <v>2018</v>
-      </c>
-      <c r="I36" s="4">
-        <v>2</v>
-      </c>
-      <c r="J36" s="4">
-        <v>25000</v>
-      </c>
-      <c r="K36" s="4">
-        <v>2</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N36" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="F37" s="37">
-        <v>3</v>
-      </c>
-      <c r="G37" s="37">
-        <v>1</v>
-      </c>
-      <c r="H37" s="37">
-        <v>2016</v>
-      </c>
-      <c r="I37" s="37">
-        <v>3</v>
-      </c>
-      <c r="J37" s="37">
+      <c r="J48" s="37">
         <v>30000</v>
       </c>
-      <c r="K37" s="37">
-        <v>2</v>
-      </c>
-      <c r="L37" s="37">
-        <v>1</v>
-      </c>
-      <c r="M37" s="37" t="s">
+      <c r="K48" s="37">
+        <v>2</v>
+      </c>
+      <c r="L48" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="N37" s="37">
+      <c r="M48" s="37">
         <v>1</v>
       </c>
     </row>
@@ -1686,4 +2048,572 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4E0589-3EAE-4539-A3CA-F6F79C9FC969}">
+  <dimension ref="H3:R61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="9" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="M9" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="M11" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J14" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J16" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="J17" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="J18" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" s="40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M23" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M24" s="43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H31" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="4">
+        <v>1</v>
+      </c>
+      <c r="J32" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="I33" s="4">
+        <v>2</v>
+      </c>
+      <c r="J33" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O33" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="I34" s="4">
+        <v>3</v>
+      </c>
+      <c r="J34" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O34" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H40" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="I41" s="4">
+        <v>1</v>
+      </c>
+      <c r="J41" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K41" s="4">
+        <v>1</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="I42" s="4">
+        <v>2</v>
+      </c>
+      <c r="J42" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K42" s="4">
+        <v>1</v>
+      </c>
+      <c r="L42" s="4">
+        <v>2</v>
+      </c>
+      <c r="M42" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="I43" s="4">
+        <v>3</v>
+      </c>
+      <c r="J43" s="38">
+        <v>46127</v>
+      </c>
+      <c r="K43" s="4">
+        <v>2</v>
+      </c>
+      <c r="L43" s="4">
+        <v>1</v>
+      </c>
+      <c r="M43" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M46" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M47" s="39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M48" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J51" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="L51" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="M51" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="N51" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="O51" s="41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J52" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="L52" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="N52" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="O52" s="39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J53" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="L53" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="M53" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="N53" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="O53" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J54" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L54" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="M54" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J55" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="L55" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="M55" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="O55" s="40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J56" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="L56" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="M56" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J57" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="M57" s="43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="M58" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="M59" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="M60" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="M61" s="43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3C67AD-0710-48F5-B545-884D6284AD2F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>